<commit_message>
cambiato theta_eG in radianti
</commit_message>
<xml_diff>
--- a/doc/rendimento pannello.xlsx
+++ b/doc/rendimento pannello.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmg\C++\repos\pv-creativity\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23471A48-DC15-40A4-9427-4EC698667193}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA929EE-99AE-4E57-B5F6-C47713AC01A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="20790" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="345" windowWidth="20790" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Martesì , ore , posizione: (Università di Bologna)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>b</t>
   </si>
@@ -39,19 +36,19 @@
     <t>Posizione del sole:</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
     <t>% rispetto al max</t>
   </si>
   <si>
-    <t>Attesa</t>
+    <t>posizione: (Università di Bologna, day 30, hour 12</t>
+  </si>
+  <si>
+    <t>S_B</t>
+  </si>
+  <si>
+    <t>S_D</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -377,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,37 +385,130 @@
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>90</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>90</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>90</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fatto controllo su beta
</commit_message>
<xml_diff>
--- a/doc/rendimento pannello.xlsx
+++ b/doc/rendimento pannello.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmg\C++\repos\pv-creativity\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA929EE-99AE-4E57-B5F6-C47713AC01A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048515C3-D9C1-4A9D-89FA-65E853538208}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="345" windowWidth="20790" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="1695" windowWidth="20790" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,12 +42,6 @@
     <t>Posizione del sole:</t>
   </si>
   <si>
-    <t>% rispetto al max</t>
-  </si>
-  <si>
-    <t>posizione: (Università di Bologna, day 30, hour 12</t>
-  </si>
-  <si>
     <t>S_B</t>
   </si>
   <si>
@@ -50,12 +50,18 @@
   <si>
     <t>S</t>
   </si>
+  <si>
+    <t>% rispetto al massimo</t>
+  </si>
+  <si>
+    <t>posizione: (Università di Bologna, day 30 (30 Gennaio), hour 12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +70,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Symbol"/>
@@ -79,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -87,13 +102,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +532,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -395,120 +540,360 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>595</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>600</v>
+      </c>
+      <c r="F4" s="14">
+        <f>E4/MAX($E$4:$E$19)</f>
+        <v>0.8771929824561403</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>15</v>
       </c>
+      <c r="C5" s="5">
+        <v>584</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>589</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" ref="F5:F19" si="0">E5/MAX($E$4:$E$19)</f>
+        <v>0.86111111111111116</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>30</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>30</v>
       </c>
+      <c r="C6" s="5">
+        <v>551</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6">
+        <v>556</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.8128654970760234</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>469</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>471</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.68859649122807021</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>15</v>
       </c>
+      <c r="C8" s="5">
+        <v>464</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>465</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.67982456140350878</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>30</v>
       </c>
+      <c r="C9" s="5">
+        <v>446</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>447</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.65350877192982459</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>302</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>302</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.44152046783625731</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
         <v>15</v>
       </c>
+      <c r="C11" s="5">
+        <v>302</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>302</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.44152046783625731</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
         <v>30</v>
       </c>
+      <c r="C12" s="5">
+        <v>302</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>302</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="0"/>
+        <v>0.44152046783625731</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>676</v>
+      </c>
+      <c r="D13" s="6">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6">
+        <v>684</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>90</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>630</v>
+      </c>
+      <c r="D14" s="6">
+        <v>32</v>
+      </c>
+      <c r="E14" s="6">
+        <v>662</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.96783625730994149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>90</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="C15" s="5">
+        <v>608</v>
+      </c>
+      <c r="D15" s="6">
+        <v>33</v>
+      </c>
+      <c r="E15" s="6">
+        <v>641</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="0"/>
+        <v>0.9371345029239766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>90</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="2">
         <v>30</v>
+      </c>
+      <c r="C16" s="5">
+        <v>542</v>
+      </c>
+      <c r="D16" s="6">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6">
+        <v>578</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="0"/>
+        <v>0.84502923976608191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>90</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5">
+        <v>436</v>
+      </c>
+      <c r="D17" s="6">
+        <v>38</v>
+      </c>
+      <c r="E17" s="6">
+        <v>474</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="0"/>
+        <v>0.69298245614035092</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2">
+        <v>60</v>
+      </c>
+      <c r="C18" s="5">
+        <v>291</v>
+      </c>
+      <c r="D18" s="6">
+        <v>40</v>
+      </c>
+      <c r="E18" s="6">
+        <v>331</v>
+      </c>
+      <c r="F18" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48391812865497075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>90</v>
+      </c>
+      <c r="B19" s="4">
+        <v>90</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <v>41</v>
+      </c>
+      <c r="E19" s="8">
+        <v>41</v>
+      </c>
+      <c r="F19" s="15">
+        <f t="shared" si="0"/>
+        <v>5.9941520467836254E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>